<commit_message>
Added more elements in ER diagram and modified queries
</commit_message>
<xml_diff>
--- a/GPE Data Dictionary (metadata).xlsx
+++ b/GPE Data Dictionary (metadata).xlsx
@@ -3,210 +3,219 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Metadata" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Página1'!$A$1:$F$69</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Metadata!$A$1:$F$77</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="93">
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Nullable</t>
+  </si>
+  <si>
+    <t>Relation To</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Applicants</t>
+  </si>
+  <si>
+    <t>student_code</t>
+  </si>
+  <si>
+    <t>char(6)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>varchar(60)</t>
+  </si>
+  <si>
+    <t>student_id</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>neighborhood</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>current_status</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>internet_access</t>
+  </si>
+  <si>
+    <t>highschool</t>
+  </si>
+  <si>
+    <t>secoundary_school</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>people_living_with_you</t>
+  </si>
+  <si>
+    <t>father_education</t>
+  </si>
+  <si>
+    <t>mother_education</t>
+  </si>
+  <si>
+    <t>tutelary_ecucation</t>
+  </si>
+  <si>
+    <t>avg_income</t>
+  </si>
+  <si>
+    <t>avg_income_percapita</t>
+  </si>
+  <si>
+    <t>father_occuparion</t>
+  </si>
+  <si>
+    <t>mother_occupation</t>
+  </si>
+  <si>
+    <t>personal_occupation</t>
+  </si>
+  <si>
+    <t>matao_residence</t>
+  </si>
+  <si>
+    <t>who_living_with_you</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>varchar(15)</t>
+  </si>
+  <si>
+    <t>vehicle</t>
+  </si>
+  <si>
+    <t>marital_status</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
+    <t>books_type</t>
+  </si>
+  <si>
+    <t>varchar(500)</t>
+  </si>
+  <si>
+    <t>movie_theather</t>
+  </si>
+  <si>
+    <t>museum</t>
+  </si>
+  <si>
+    <t>additional_courses</t>
+  </si>
+  <si>
+    <t>career</t>
+  </si>
+  <si>
+    <t>study_room</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>computers</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>smartphones</t>
+  </si>
+  <si>
+    <t>parents_conversation</t>
+  </si>
+  <si>
+    <t>Entrance_Exame</t>
+  </si>
+  <si>
+    <t>student_code in Applicants table</t>
+  </si>
+  <si>
+    <t>geography</t>
+  </si>
+  <si>
+    <t>decimal(5,4)</t>
+  </si>
+  <si>
+    <t>biology</t>
+  </si>
+  <si>
+    <t>chemistry</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>portuguese</t>
+  </si>
+  <si>
+    <t>literature</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>interdisplinary</t>
+  </si>
   <si>
     <t>Students</t>
   </si>
   <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Data Type</t>
-  </si>
-  <si>
-    <t>Nullable</t>
-  </si>
-  <si>
-    <t>Relation To</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Applicants</t>
-  </si>
-  <si>
-    <t>student_code</t>
-  </si>
-  <si>
-    <t>char(6)</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>varchar(60)</t>
-  </si>
-  <si>
-    <t>student_id</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>neighborhood</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>phone_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>current_status</t>
-  </si>
-  <si>
-    <t>varchar(100)</t>
-  </si>
-  <si>
-    <t>internet_access</t>
-  </si>
-  <si>
-    <t>highschool</t>
-  </si>
-  <si>
-    <t>secoundary_school</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>people_living_with_you</t>
-  </si>
-  <si>
-    <t>father_education</t>
-  </si>
-  <si>
-    <t>mother_education</t>
-  </si>
-  <si>
-    <t>tutelary_ecucation</t>
-  </si>
-  <si>
-    <t>avg_income</t>
-  </si>
-  <si>
-    <t>avg_income_percapita</t>
-  </si>
-  <si>
-    <t>father_occuparion</t>
-  </si>
-  <si>
-    <t>mother_occupation</t>
-  </si>
-  <si>
-    <t>personal_occupation</t>
-  </si>
-  <si>
-    <t>matao_residence</t>
-  </si>
-  <si>
-    <t>who_living_with_you</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>varchar(15)</t>
-  </si>
-  <si>
-    <t>vehicle</t>
-  </si>
-  <si>
-    <t>marital_status</t>
-  </si>
-  <si>
-    <t>books</t>
-  </si>
-  <si>
-    <t>books_type</t>
-  </si>
-  <si>
-    <t>varchar(500)</t>
-  </si>
-  <si>
-    <t>movie_theather</t>
-  </si>
-  <si>
-    <t>museum</t>
-  </si>
-  <si>
-    <t>additional_courses</t>
-  </si>
-  <si>
-    <t>career</t>
-  </si>
-  <si>
-    <t>study_room</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>computers</t>
-  </si>
-  <si>
-    <t>varchar(30)</t>
-  </si>
-  <si>
-    <t>smartphones</t>
-  </si>
-  <si>
-    <t>parents_conversation</t>
-  </si>
-  <si>
-    <t>Exam_Entrance</t>
-  </si>
-  <si>
-    <t>student_code in Applicants tab</t>
-  </si>
-  <si>
-    <t>chemistry</t>
-  </si>
-  <si>
-    <t>decimal(5,4)</t>
-  </si>
-  <si>
-    <t>history</t>
-  </si>
-  <si>
-    <t>math</t>
-  </si>
-  <si>
-    <t>physics</t>
-  </si>
-  <si>
-    <t>portuguese</t>
-  </si>
-  <si>
-    <t>literature</t>
-  </si>
-  <si>
-    <t>english</t>
-  </si>
-  <si>
-    <t>interdisplinary</t>
-  </si>
-  <si>
     <t>NSE</t>
   </si>
   <si>
@@ -228,7 +237,7 @@
     <t>Exams</t>
   </si>
   <si>
-    <t>student_code in Students tab</t>
+    <t>student_code in Students table</t>
   </si>
   <si>
     <t>exame_number</t>
@@ -240,7 +249,7 @@
     <t>volunteer_ids</t>
   </si>
   <si>
-    <t>volunteer_id in Students tab</t>
+    <t>volunteer_id in Students table</t>
   </si>
   <si>
     <t>name</t>
@@ -252,6 +261,9 @@
     <t xml:space="preserve">team_id </t>
   </si>
   <si>
+    <t>role_id</t>
+  </si>
+  <si>
     <t>Team</t>
   </si>
   <si>
@@ -261,7 +273,25 @@
     <t>team_ids</t>
   </si>
   <si>
-    <t>team_id in Volunteers tab</t>
+    <t>team_id in Volunteers table</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>role_ids</t>
+  </si>
+  <si>
+    <t>role_id in  Volunteers table</t>
+  </si>
+  <si>
+    <t>role_name</t>
+  </si>
+  <si>
+    <t>role_description</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -1111,6 +1141,7 @@
       <c r="D39" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E39" s="3"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
@@ -1125,6 +1156,7 @@
       <c r="D40" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E40" s="3"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
@@ -1212,27 +1244,24 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>56</v>
@@ -1243,97 +1272,100 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>67</v>
+        <v>9</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>56</v>
@@ -1341,13 +1373,14 @@
       <c r="D55" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E55" s="2"/>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>56</v>
@@ -1355,13 +1388,14 @@
       <c r="D56" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E56" s="2"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>56</v>
@@ -1372,10 +1406,10 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>56</v>
@@ -1386,10 +1420,10 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>56</v>
@@ -1400,10 +1434,10 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>56</v>
@@ -1414,13 +1448,13 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>9</v>
@@ -1431,16 +1465,13 @@
         <v>73</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="63">
@@ -1448,10 +1479,10 @@
         <v>73</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>9</v>
@@ -1462,13 +1493,13 @@
         <v>73</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65">
@@ -1476,7 +1507,7 @@
         <v>73</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>13</v>
@@ -1487,49 +1518,52 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>67</v>
+        <v>9</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>81</v>
@@ -1540,12 +1574,129 @@
       <c r="D69" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E69" s="2" t="s">
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="C70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E77" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$F$69"/>
+  <autoFilter ref="$A$1:$F$77"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected some queries to create tables
</commit_message>
<xml_diff>
--- a/GPE Data Dictionary (metadata).xlsx
+++ b/GPE Data Dictionary (metadata).xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Metadata" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Metadata!$A$1:$F$77</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Metadata!$A$1:$F$79</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="95">
   <si>
     <t>Tables</t>
   </si>
@@ -36,21 +36,24 @@
     <t>Applicants</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>varchar(60)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>student_code</t>
   </si>
   <si>
     <t>char(6)</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
-    <t>varchar(60)</t>
-  </si>
-  <si>
     <t>student_id</t>
   </si>
   <si>
@@ -78,6 +81,9 @@
     <t>varchar(100)</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>internet_access</t>
   </si>
   <si>
@@ -225,9 +231,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>end_date</t>
   </si>
   <si>
@@ -252,10 +255,13 @@
     <t>volunteer_id in Students table</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>degree</t>
+  </si>
+  <si>
+    <t>university</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
   </si>
   <si>
     <t xml:space="preserve">team_id </t>
@@ -604,7 +610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -618,7 +624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -632,7 +638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -640,27 +646,27 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" hidden="1">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -668,13 +674,13 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -682,13 +688,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -696,254 +702,254 @@
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2" t="s">
+    </row>
+    <row r="9" hidden="1">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+    </row>
+    <row r="10" hidden="1">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" hidden="1">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" hidden="1">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" hidden="1">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" hidden="1">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" hidden="1">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" hidden="1">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" hidden="1">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" hidden="1">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" hidden="1">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" hidden="1">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" hidden="1">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" hidden="1">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" hidden="1">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" hidden="1">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" hidden="1">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" hidden="1">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -951,55 +957,55 @@
         <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" hidden="1">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" hidden="1">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" hidden="1">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" hidden="1">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1007,69 +1013,69 @@
         <v>43</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" hidden="1">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" hidden="1">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" hidden="1">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" hidden="1">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" hidden="1">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1080,10 +1086,10 @@
         <v>50</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" hidden="1">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1091,67 +1097,66 @@
         <v>51</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" hidden="1">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" hidden="1">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>9</v>
@@ -1160,27 +1165,28 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E41" s="3"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>9</v>
@@ -1188,13 +1194,13 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>9</v>
@@ -1202,13 +1208,13 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>9</v>
@@ -1216,13 +1222,13 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>9</v>
@@ -1230,13 +1236,13 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>9</v>
@@ -1244,13 +1250,13 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>9</v>
@@ -1258,132 +1264,131 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" hidden="1">
       <c r="A50" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51">
+    </row>
+    <row r="51" hidden="1">
       <c r="A51" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" hidden="1">
+      <c r="A52" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" hidden="1">
       <c r="A53" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" hidden="1">
       <c r="A54" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C54" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>9</v>
@@ -1392,27 +1397,28 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E57" s="2"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>9</v>
@@ -1420,13 +1426,13 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>9</v>
@@ -1434,13 +1440,13 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>9</v>
@@ -1448,13 +1454,13 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>9</v>
@@ -1462,13 +1468,13 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>9</v>
@@ -1476,13 +1482,13 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>9</v>
@@ -1490,213 +1496,248 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" hidden="1">
+      <c r="A67" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68">
+    </row>
+    <row r="68" hidden="1">
       <c r="A68" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" hidden="1">
+      <c r="A69" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="2" t="s">
+      <c r="C69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" hidden="1">
+      <c r="A70" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" hidden="1">
+      <c r="A71" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" hidden="1">
+      <c r="A72" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" hidden="1">
+      <c r="A73" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D73" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" hidden="1">
       <c r="A74" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" hidden="1">
+      <c r="A75" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="2" t="s">
+      <c r="C75" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" hidden="1">
+      <c r="A76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C76" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="2" t="s">
+    </row>
+    <row r="77" hidden="1">
+      <c r="A77" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="2"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C77" s="2" t="s">
+    </row>
+    <row r="78" hidden="1">
+      <c r="A78" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E77" s="2"/>
+      <c r="C78" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" hidden="1">
+      <c r="A79" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$F$77"/>
+  <autoFilter ref="$A$1:$F$79">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Exams"/>
+        <filter val="Entrance_Exame"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more columns in some tables
</commit_message>
<xml_diff>
--- a/GPE Data Dictionary (metadata).xlsx
+++ b/GPE Data Dictionary (metadata).xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Metadata" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Metadata!$A$1:$F$79</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Metadata!$A$1:$F$81</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="96">
   <si>
     <t>Tables</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>role_id</t>
+  </si>
+  <si>
+    <t>varchar(35)</t>
   </si>
   <si>
     <t>Team</t>
@@ -1131,7 +1134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="1">
       <c r="A39" s="2" t="s">
         <v>55</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="1">
       <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
@@ -1163,7 +1166,7 @@
       </c>
       <c r="E40" s="3"/>
     </row>
-    <row r="41">
+    <row r="41" hidden="1">
       <c r="A41" s="2" t="s">
         <v>55</v>
       </c>
@@ -1178,7 +1181,7 @@
       </c>
       <c r="E41" s="3"/>
     </row>
-    <row r="42">
+    <row r="42" hidden="1">
       <c r="A42" s="2" t="s">
         <v>55</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="1">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="1">
       <c r="A44" s="2" t="s">
         <v>55</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="1">
       <c r="A45" s="2" t="s">
         <v>55</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="1">
       <c r="A46" s="2" t="s">
         <v>55</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="1">
       <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="1">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="1">
       <c r="A55" s="2" t="s">
         <v>74</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="1">
       <c r="A56" s="2" t="s">
         <v>74</v>
       </c>
@@ -1395,7 +1398,7 @@
       </c>
       <c r="E56" s="2"/>
     </row>
-    <row r="57">
+    <row r="57" hidden="1">
       <c r="A57" s="2" t="s">
         <v>74</v>
       </c>
@@ -1410,7 +1413,7 @@
       </c>
       <c r="E57" s="2"/>
     </row>
-    <row r="58">
+    <row r="58" hidden="1">
       <c r="A58" s="2" t="s">
         <v>74</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="1">
       <c r="A59" s="2" t="s">
         <v>74</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="1">
       <c r="A60" s="2" t="s">
         <v>74</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="1">
       <c r="A61" s="2" t="s">
         <v>74</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="1">
       <c r="A62" s="2" t="s">
         <v>74</v>
       </c>
@@ -1480,7 +1483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="1">
       <c r="A63" s="2" t="s">
         <v>74</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="1">
       <c r="A64" s="2" t="s">
         <v>74</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="1">
       <c r="A65" s="2" t="s">
         <v>74</v>
       </c>
@@ -1522,7 +1525,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="1">
       <c r="A66" s="2" t="s">
         <v>74</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" hidden="1">
+    <row r="67">
       <c r="A67" s="2" t="s">
         <v>77</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" hidden="1">
+    <row r="68">
       <c r="A68" s="2" t="s">
         <v>77</v>
       </c>
@@ -1567,7 +1570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" hidden="1">
+    <row r="69">
       <c r="A69" s="2" t="s">
         <v>77</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" hidden="1">
+    <row r="70">
       <c r="A70" s="2" t="s">
         <v>77</v>
       </c>
@@ -1595,7 +1598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" hidden="1">
+    <row r="71">
       <c r="A71" s="2" t="s">
         <v>77</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" hidden="1">
+    <row r="72">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
@@ -1623,118 +1626,145 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" hidden="1">
+    <row r="73">
       <c r="A73" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="74" hidden="1">
+    <row r="74">
       <c r="A74" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="75" hidden="1">
-      <c r="A75" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" hidden="1">
-      <c r="A76" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" hidden="1">
       <c r="A77" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="78" hidden="1">
       <c r="A78" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="2"/>
     </row>
     <row r="79" hidden="1">
       <c r="A79" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" hidden="1">
+      <c r="A80" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" hidden="1">
+      <c r="A81" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E79" s="2"/>
+      <c r="C81" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$F$79">
+  <autoFilter ref="$A$1:$F$81">
     <filterColumn colId="0">
       <filters>
-        <filter val="Exams"/>
-        <filter val="Entrance_Exame"/>
+        <filter val="Volunteers"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>